<commit_message>
feat:GUI redone using flet - It remains to make the download buttons work and the select directory button needs to save the selected directory in a control variable - The control variables also need to work
</commit_message>
<xml_diff>
--- a/config/languages.xlsx
+++ b/config/languages.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raulc\Desktop\Dev\Apps\Apps_Python\Proyectos\EasyViewer\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7C17FBB-3B90-413A-B3E2-8C5F08A4EFE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE377F9-5C5A-48A6-819C-912AA0D36476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>Español</t>
   </si>
@@ -28,18 +28,6 @@
     <t>English</t>
   </si>
   <si>
-    <t>Introduce la URL del video a descargar</t>
-  </si>
-  <si>
-    <t>Enter the URL of the video to download</t>
-  </si>
-  <si>
-    <t>¿Donde quieres guardar el video?</t>
-  </si>
-  <si>
-    <t>Where do you want to save the video?</t>
-  </si>
-  <si>
     <t>Seleccionar ubicación</t>
   </si>
   <si>
@@ -58,42 +46,12 @@
     <t>Download audio</t>
   </si>
   <si>
-    <t>Progreso de la descarga</t>
-  </si>
-  <si>
-    <t>Download progress</t>
-  </si>
-  <si>
     <t>¿Está seguro de que desea salir?</t>
   </si>
   <si>
     <t>Are you sure you want to go out?</t>
   </si>
   <si>
-    <t>Si, salir de la app</t>
-  </si>
-  <si>
-    <t>Yes, exit the app</t>
-  </si>
-  <si>
-    <t>No, solo minimizar</t>
-  </si>
-  <si>
-    <t>No, just minimize</t>
-  </si>
-  <si>
-    <t>Cancelar, permanecer en la app</t>
-  </si>
-  <si>
-    <t>Cancel, stay in the app</t>
-  </si>
-  <si>
-    <t>Salir</t>
-  </si>
-  <si>
-    <t>Exit</t>
-  </si>
-  <si>
     <t>Contacto</t>
   </si>
   <si>
@@ -128,13 +86,43 @@
   </si>
   <si>
     <t>The URL is not from YouTube</t>
+  </si>
+  <si>
+    <t>Si</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Confirmación cierre</t>
+  </si>
+  <si>
+    <t>Closing confirmation</t>
+  </si>
+  <si>
+    <t>Select directory</t>
+  </si>
+  <si>
+    <t>Selecciona directorio</t>
+  </si>
+  <si>
+    <t>URL del video</t>
+  </si>
+  <si>
+    <t>Video URL</t>
+  </si>
+  <si>
+    <t>Directorio para el video o el audio del video</t>
+  </si>
+  <si>
+    <t>Directory for video or audio in video</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,12 +134,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial Black"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
@@ -188,15 +170,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -507,16 +486,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.42578125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
@@ -544,7 +523,7 @@
       </c>
     </row>
     <row r="4" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -560,115 +539,99 @@
       </c>
     </row>
     <row r="6" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>10</v>
+      <c r="A6" s="2" t="s">
+        <v>22</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>18</v>
+      <c r="A10" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>26</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="B17" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Added contact form - The user selects from a dropdown the appropriate social network to contact me - After obtaining the social network selected by the user of the dropdown, it is used as a key to obtain the link to the social network selects from a dictionary called "social_networks", and that link obtained from the dictionary opens in a new browser tab using the function "open_new_tab" of the module "webbrowser"
</commit_message>
<xml_diff>
--- a/config/languages.xlsx
+++ b/config/languages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raulc\Desktop\Dev\Apps\Apps_Python\Proyectos\EasyViewer\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE377F9-5C5A-48A6-819C-912AA0D36476}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8F1B9D-04D9-48A8-8210-5D7DFE515C74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>Español</t>
   </si>
@@ -116,6 +116,12 @@
   </si>
   <si>
     <t>Directory for video or audio in video</t>
+  </si>
+  <si>
+    <t>Redes sociales</t>
+  </si>
+  <si>
+    <t>Social networks</t>
   </si>
 </sst>
 </file>
@@ -486,10 +492,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,6 +640,14 @@
         <v>31</v>
       </c>
     </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Fix: Corrected error in downloaded audio extension and file name. - Now the file location and download name are obtained when executing the corresponding function in the "download.py" file. - Validations have been added in the "interact_api_pytube.py" file to prevent the file name from having two consecutive colons if the title ends with a period, and to remove the "|" character from the title to avoid issues on Windows when saving the file.
</commit_message>
<xml_diff>
--- a/config/languages.xlsx
+++ b/config/languages.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raulc\Desktop\Dev\Apps\Apps_Python\Proyectos\EasyViewer\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8F1B9D-04D9-48A8-8210-5D7DFE515C74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70B34FDF-857A-42F4-99CC-D77EE356B03B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>Español</t>
   </si>
@@ -122,13 +122,21 @@
   </si>
   <si>
     <t>Social networks</t>
+  </si>
+  <si>
+    <t>There was a problem trying to get the video.
+Please try again</t>
+  </si>
+  <si>
+    <t>Hubo un problema al intentar obtener el video.
+Por favor inténtelo de nuevo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,6 +155,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -176,16 +192,25 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -492,161 +517,172 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B18"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="45.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="41.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="70.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="54.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="5" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="5" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="5" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="5" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="6" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="6" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="A16" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="6" t="s">
         <v>33</v>
       </c>
+    </row>
+    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B23" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: Implementation of automatic update of the app from the latest version available on GitHub. - The "pygithub" library is used to connect to the GitHub API and you get the download link and the version of the latest release. - If the user's version is lower than the release, a dialog box is displayed indicating the need to update the app and if it gives to update it is downloaded and installed automatically. - If the user already has the latest version, a dialog box is displayed informing him - Note: The current implementation only obtains the link and performs version comparison; download and installation logic is not yet implemented
</commit_message>
<xml_diff>
--- a/config/languages.xlsx
+++ b/config/languages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raulc\Desktop\Dev\Apps\Apps_Python\Proyectos\EasyViewer\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70B34FDF-857A-42F4-99CC-D77EE356B03B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F71408D-DA43-4586-9B3A-016ACB53939A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,11 +16,12 @@
     <sheet name="Idiomas" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
   <si>
     <t>Español</t>
   </si>
@@ -124,12 +125,32 @@
     <t>Social networks</t>
   </si>
   <si>
-    <t>There was a problem trying to get the video.
+    <t>Habido un problema mientras se intentaba obtener el video.
+Por favor inténtelo de nuevo</t>
+  </si>
+  <si>
+    <t>There was a problem while trying to get the video.
 Please try again</t>
   </si>
   <si>
-    <t>Hubo un problema al intentar obtener el video.
-Por favor inténtelo de nuevo</t>
+    <t>Hay una nueva version disponible.
+¿Quieres actualizar a la última versión?</t>
+  </si>
+  <si>
+    <t>You've the latest version available</t>
+  </si>
+  <si>
+    <t>There's a new version available. 
+Do you wanna update to the latest version?</t>
+  </si>
+  <si>
+    <t>Tienes la ultima versión disponible</t>
+  </si>
+  <si>
+    <t>Actualizar mas tarde</t>
+  </si>
+  <si>
+    <t>Update later</t>
   </si>
 </sst>
 </file>
@@ -519,8 +540,8 @@
   </sheetPr>
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,10 +696,34 @@
     </row>
     <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>34</v>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix: Resolve KeyError in update dialog title - Accessing row 21 in the excel file for the update dialog title caused a KeyError due to its accidental deletion. - The issue was fixed by recreating the missing row in the excel file.
</commit_message>
<xml_diff>
--- a/config/languages.xlsx
+++ b/config/languages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raulc\Desktop\Dev\Apps\Apps_Python\Proyectos\EasyViewer\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F71408D-DA43-4586-9B3A-016ACB53939A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C5BBAA-22EE-4A27-8DD3-7EE974599B0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,12 +16,11 @@
     <sheet name="Idiomas" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
   <si>
     <t>Español</t>
   </si>
@@ -144,20 +143,26 @@
 Do you wanna update to the latest version?</t>
   </si>
   <si>
-    <t>Tienes la ultima versión disponible</t>
-  </si>
-  <si>
     <t>Actualizar mas tarde</t>
   </si>
   <si>
     <t>Update later</t>
+  </si>
+  <si>
+    <t>Actualizar aplicación</t>
+  </si>
+  <si>
+    <t>Update app</t>
+  </si>
+  <si>
+    <t>Tienes la última versión disponible</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -176,14 +181,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -218,9 +215,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -231,6 +225,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -540,8 +537,8 @@
   </sheetPr>
   <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,183 +548,188 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="5" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="5" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="A19" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="B22" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="6" t="s">
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B23" s="2"/>
+      <c r="B23" s="6" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
refactor: Remove automatic update functionality - This commit removes the automatic update functionality from the app. After careful consideration, I've decided to remove it for the following reasons:
1) Unnecessary: Given the simplicity of the app, an automatic update system is not essential at this point. I may consider adding it in the future if it becomes necessary.

2) Complexity: Implementing the automatic update system proved to be too complicated, even though I managed to create a base. There were issues with installation, and the system didn't always work reliably.
</commit_message>
<xml_diff>
--- a/config/languages.xlsx
+++ b/config/languages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raulc\Desktop\Dev\Apps\Apps_Python\Proyectos\EasyViewer\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C5BBAA-22EE-4A27-8DD3-7EE974599B0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E90381-42EC-4760-9157-81AB4F23EB99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>Español</t>
   </si>
@@ -130,32 +130,6 @@
   <si>
     <t>There was a problem while trying to get the video.
 Please try again</t>
-  </si>
-  <si>
-    <t>Hay una nueva version disponible.
-¿Quieres actualizar a la última versión?</t>
-  </si>
-  <si>
-    <t>You've the latest version available</t>
-  </si>
-  <si>
-    <t>There's a new version available. 
-Do you wanna update to the latest version?</t>
-  </si>
-  <si>
-    <t>Actualizar mas tarde</t>
-  </si>
-  <si>
-    <t>Update later</t>
-  </si>
-  <si>
-    <t>Actualizar aplicación</t>
-  </si>
-  <si>
-    <t>Update app</t>
-  </si>
-  <si>
-    <t>Tienes la última versión disponible</t>
   </si>
 </sst>
 </file>
@@ -210,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -225,9 +199,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -538,7 +509,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,36 +671,20 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>38</v>
-      </c>
+      <c r="A20" s="5"/>
+      <c r="B20" s="5"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>40</v>
-      </c>
+      <c r="A22" s="5"/>
+      <c r="B22" s="5"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>42</v>
-      </c>
+      <c r="A23" s="5"/>
+      <c r="B23" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
feat: Initial implementation of the automatic application updater - I've started the implementation of an automatic updater of the application. The current code configures the necessary structure and retrieves the information from the latest version of GitHub.
- The "Update" class provides methods for retrieving the latest version and the current version of the user"s application. The "is_new_release_available" method compares these versions to determine if an update is available.

- The "update" method is a placeholder and will be further developed to handle the actual update process, including downloading and replacing the app files.

- This initial deployment lays the foundation for the automatic updater of the application, and work will continue to complete the update functionality
</commit_message>
<xml_diff>
--- a/config/languages.xlsx
+++ b/config/languages.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raulc\Desktop\Dev\Apps\Apps_Python\Proyectos\EasyViewer\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E90381-42EC-4760-9157-81AB4F23EB99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{921F662C-D1F5-49FE-889F-64D185A057B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
   <si>
     <t>Español</t>
   </si>
@@ -46,12 +46,6 @@
     <t>Download audio</t>
   </si>
   <si>
-    <t>¿Está seguro de que desea salir?</t>
-  </si>
-  <si>
-    <t>Are you sure you want to go out?</t>
-  </si>
-  <si>
     <t>Contacto</t>
   </si>
   <si>
@@ -119,9 +113,6 @@
   </si>
   <si>
     <t>Redes sociales</t>
-  </si>
-  <si>
-    <t>Social networks</t>
   </si>
   <si>
     <t>Habido un problema mientras se intentaba obtener el video.
@@ -130,6 +121,33 @@
   <si>
     <t>There was a problem while trying to get the video.
 Please try again</t>
+  </si>
+  <si>
+    <t>Are you sure you wanna go out?</t>
+  </si>
+  <si>
+    <t>¿Estás seguro de que quieres salir?</t>
+  </si>
+  <si>
+    <t>Social Media</t>
+  </si>
+  <si>
+    <t>Hay una nueva versión disponible</t>
+  </si>
+  <si>
+    <t>A new version is available</t>
+  </si>
+  <si>
+    <t>¿Quieres actualizar a la ultima versión?</t>
+  </si>
+  <si>
+    <t>Do you wanna update to the latest version?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Más tarde </t>
+  </si>
+  <si>
+    <t>Later</t>
   </si>
 </sst>
 </file>
@@ -509,7 +527,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,34 +570,34 @@
     </row>
     <row r="5" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -587,12 +605,12 @@
         <v>0</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>1</v>
@@ -600,87 +618,99 @@
     </row>
     <row r="11" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="5"/>
+      <c r="A20" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
+      <c r="A21" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="5"/>
+      <c r="A22" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>

</xml_diff>

<commit_message>
feat: Automatic update checking option - Added a checkbox in the taskbar (top of the window) to control the automatic update checking functionality. When the checkbox is checked, the application will automatically check for available updates. Conversely, if it's unchecked, the user can manually trigger the update check.
- Implemented a control variable called "checkbox_value" to store the value of the checkbox. This variable is used to preserve the user's preference for future application sessions.

- To persist the user's preference, the "checkbox_value" is stored in the client's storage using the "checkbox" key. This ensures that the chosen setting is loaded each time the application is started.

- This approach provides users with flexibility and control over the update process, allowing them to choose the preferred update checking method according to their needs and preferences.
</commit_message>
<xml_diff>
--- a/config/languages.xlsx
+++ b/config/languages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raulc\Desktop\Dev\Apps\Apps_Python\Proyectos\EasyViewer\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{921F662C-D1F5-49FE-889F-64D185A057B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8591816E-D002-4524-942B-1FCB049D26D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
   <si>
     <t>Español</t>
   </si>
@@ -115,14 +115,6 @@
     <t>Redes sociales</t>
   </si>
   <si>
-    <t>Habido un problema mientras se intentaba obtener el video.
-Por favor inténtelo de nuevo</t>
-  </si>
-  <si>
-    <t>There was a problem while trying to get the video.
-Please try again</t>
-  </si>
-  <si>
     <t>Are you sure you wanna go out?</t>
   </si>
   <si>
@@ -148,6 +140,26 @@
   </si>
   <si>
     <t>Later</t>
+  </si>
+  <si>
+    <t>Comprobar actualizaciones automáticamente</t>
+  </si>
+  <si>
+    <t>Check for updates automatically</t>
+  </si>
+  <si>
+    <t>Versión Actualizada</t>
+  </si>
+  <si>
+    <t>¡Felicidades! Estás utilizando la última versión de la aplicación. 
+No es necesario realizar ninguna actualización en este momento.</t>
+  </si>
+  <si>
+    <t>Updated Version</t>
+  </si>
+  <si>
+    <t>Congratulations! You are using the latest version of the app. 
+No update is required at this time.</t>
   </si>
 </sst>
 </file>
@@ -524,10 +536,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B23"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,10 +582,10 @@
     </row>
     <row r="5" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -677,30 +689,30 @@
         <v>30</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="5" t="s">
         <v>39</v>
       </c>
     </row>
@@ -713,8 +725,20 @@
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="5"/>
+      <c r="A23" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
chore: Improve user-friendly download error message - Previously, the download error message displayed the raw error message provided by "pytube". However, this message may not be easily understandable to non-developer users, leading to confusion.
- To improve the user experience, I've modified the download error message to be more friendly for the non-developer user

- By providing a clear and understandable error message, we aim to improve the usability of the app
</commit_message>
<xml_diff>
--- a/config/languages.xlsx
+++ b/config/languages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\raulc\Desktop\Dev\Apps\Apps_Python\Proyectos\EasyViewer\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8591816E-D002-4524-942B-1FCB049D26D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2F7A006-EFB6-4DCA-948D-9F14C9C62D69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
   <si>
     <t>Español</t>
   </si>
@@ -160,6 +160,16 @@
   <si>
     <t>Congratulations! You are using the latest version of the app. 
 No update is required at this time.</t>
+  </si>
+  <si>
+    <t>Algo ha ido mal. 
+Por favor, inténtalo de nuevo más tarde. 
+Si el problema persiste, contacta conmigo a través de mis redes sociales</t>
+  </si>
+  <si>
+    <t>Something has gone wrong. 
+Please try again later. 
+If the problem persists, contact me through my social networks</t>
   </si>
 </sst>
 </file>
@@ -536,10 +546,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,6 +750,14 @@
         <v>45</v>
       </c>
     </row>
+    <row r="25" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>